<commit_message>
BubbleSheet => Mon Dec 16 21:33:59 EET 2019
</commit_message>
<xml_diff>
--- a/output/Sheet.xlsx
+++ b/output/Sheet.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -380,6 +380,309 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4">
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>No answer</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Can't load image</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Error in the system , error (0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Error in the system , error (0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Error in the system , error (0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Error in the system , error (0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>No answer</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Error in the system , error (0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Error in the system , error (0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Error in the system , error (0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>No answer</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>No answer</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>No answer</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>No answer</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Can't load image</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>No answer</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="n">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
BubbleSheet => Mon Dec 16 23:35:02 EET 2019
</commit_message>
<xml_diff>
--- a/output/Sheet.xlsx
+++ b/output/Sheet.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -683,6 +683,279 @@
         <v>8</v>
       </c>
     </row>
+    <row r="54">
+      <c r="B54" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Can't load image</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Can't load image</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Can't load image</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Error in the system , error (0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="B82" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="B84" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Can't load image</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="B87" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="B89" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="B90" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="B91" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="B92" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="B93" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="B95" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="B96" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="B97" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="B98" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="B99" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="B100" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="B102" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="B104" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="B105" t="n">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>